<commit_message>
ISP20220288 - 調整 1. UI上的Released Date要改成Report Date 2. .Excel加上欄位 3. 日期的框框寬度加長
</commit_message>
<xml_diff>
--- a/Quality/Quality/XLT/Search List.xlsx
+++ b/Quality/Quality/XLT/Search List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Type</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -58,6 +58,14 @@
   </si>
   <si>
     <t>Style#</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Received Date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Report Date</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -451,20 +459,18 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="9" width="20.625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="20.625" style="4" customWidth="1"/>
-    <col min="11" max="16384" width="9" style="2"/>
+    <col min="10" max="12" width="20.625" style="4" customWidth="1"/>
+    <col min="13" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -493,6 +499,12 @@
         <v>7</v>
       </c>
       <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ISP20230142 - 工廠端Quality 的Search List，To Excel加上Line欄位及Technician Name
</commit_message>
<xml_diff>
--- a/Quality/Quality/XLT/Search List.xlsx
+++ b/Quality/Quality/XLT/Search List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Type</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -66,6 +66,14 @@
   </si>
   <si>
     <t>Report Date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Line</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Technician Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -459,18 +467,19 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="9" width="20.625" style="2" customWidth="1"/>
-    <col min="10" max="12" width="20.625" style="4" customWidth="1"/>
-    <col min="13" max="16384" width="9" style="2"/>
+    <col min="1" max="10" width="20.625" style="2" customWidth="1"/>
+    <col min="11" max="13" width="20.625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="20.625" style="2" customWidth="1"/>
+    <col min="15" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -493,19 +502,25 @@
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>6</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>